<commit_message>
geomorphology and water samples updates
</commit_message>
<xml_diff>
--- a/Geomorphology/Atenas/Antenas_Notes.xlsx
+++ b/Geomorphology/Atenas/Antenas_Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/kriddie_ad_unc_edu/Documents/Ecuador2021/Ecuador2021/Geomorphology/Atenas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whitm\OneDrive - University of North Carolina at Chapel Hill\Ecuador2021\Ecuador2021\Geomorphology\Atenas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="424" documentId="8_{19832570-8386-4879-B1A8-58ACBC980CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEB06932-3895-4A80-80D6-A82F9F018970}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F1B0D5-DE63-4FBC-A48B-F94B02F5401F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AE8C079-483A-41C0-9A73-DDACF807A788}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AE8C079-483A-41C0-9A73-DDACF807A788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,26 +619,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D24120F-C55C-4FCB-858D-EF02DE86CF7F}">
   <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="N112" sqref="N112"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44389</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -646,7 +647,7 @@
         <v>0.43472222222222223</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -663,7 +664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -671,18 +672,18 @@
         <v>0.43472222222222223</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -711,7 +712,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -737,7 +738,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4</v>
       </c>
@@ -766,7 +767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5</v>
       </c>
@@ -777,7 +778,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>10</v>
       </c>
@@ -788,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -817,7 +818,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14.1</v>
       </c>
@@ -843,7 +844,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -857,7 +858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>20</v>
       </c>
@@ -868,7 +869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>25</v>
       </c>
@@ -879,7 +880,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>30</v>
       </c>
@@ -890,7 +891,7 @@
         <v>2.54</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>35</v>
       </c>
@@ -901,7 +902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>40</v>
       </c>
@@ -912,7 +913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>45</v>
       </c>
@@ -923,7 +924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>50</v>
       </c>
@@ -934,7 +935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>55</v>
       </c>
@@ -945,7 +946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>60</v>
       </c>
@@ -959,7 +960,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>65</v>
       </c>
@@ -988,7 +989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>70</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>75</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>80</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>85</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>87.5</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>90</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>91</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>95</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>100</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>105</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>110</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>115</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>115.1</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>120</v>
       </c>
@@ -1196,7 +1197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>125</v>
       </c>
@@ -1207,7 +1208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>126</v>
       </c>
@@ -1218,7 +1219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>130</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>135</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>140</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>140.5</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>145</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>150</v>
       </c>
@@ -1317,7 +1318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>159</v>
       </c>
@@ -1331,7 +1332,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>155</v>
       </c>
@@ -1342,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>156</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>160</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>165</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>170</v>
       </c>
@@ -1428,7 +1429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>175</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>180</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>185</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>190</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>195</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>198</v>
       </c>
@@ -1512,7 +1513,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>200</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>204</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>205</v>
       </c>
@@ -1548,7 +1549,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>210</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>215</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>218</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>220</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>225</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>230</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>235</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>240</v>
       </c>
@@ -1669,7 +1670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>241</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>245</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>250</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>254</v>
       </c>
@@ -1731,7 +1732,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>258</v>
       </c>
@@ -1760,7 +1761,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>260</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>265</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>270</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>275</v>
       </c>
@@ -1819,7 +1820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>280</v>
       </c>
@@ -1830,7 +1831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>282</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>285</v>
       </c>
@@ -1867,7 +1868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>290</v>
       </c>
@@ -1878,7 +1879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>295</v>
       </c>
@@ -1889,7 +1890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>300</v>
       </c>
@@ -1900,7 +1901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>305</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>310</v>
       </c>
@@ -1922,7 +1923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>315</v>
       </c>
@@ -1948,7 +1949,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>316</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>320</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>325</v>
       </c>
@@ -1984,7 +1985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>330</v>
       </c>
@@ -1995,7 +1996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>332</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>335</v>
       </c>
@@ -2035,7 +2036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>340</v>
       </c>
@@ -2046,7 +2047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>345</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>350</v>
       </c>
@@ -2089,7 +2090,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>355</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>360</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>365</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>410</v>
       </c>
@@ -2166,7 +2167,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>416</v>
       </c>
@@ -2210,7 +2211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>420</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>425</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>430</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>435</v>
       </c>
@@ -2254,7 +2255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>440</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>445</v>
       </c>
@@ -2276,7 +2277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>450</v>
       </c>
@@ -2287,7 +2288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>455</v>
       </c>
@@ -2313,7 +2314,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>460</v>
       </c>

</xml_diff>